<commit_message>
file : add balancing 견적 및 3d model
</commit_message>
<xml_diff>
--- a/Files/Banlacing 견적.xlsx
+++ b/Files/Banlacing 견적.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juhyu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sagi_JJU D\Git_Fork\Balancer\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44E7B774-9850-4ECD-925E-377378F2B3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47F0811-BB87-4B12-93CE-E0AD1C1BC76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="2445" windowWidth="18765" windowHeight="11505" xr2:uid="{E1DD097F-CCCD-47D4-AF95-9B580DA036E3}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{E1DD097F-CCCD-47D4-AF95-9B580DA036E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>방식 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,10 @@
   </si>
   <si>
     <t>합계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새방식</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,14 +391,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
@@ -448,8 +449,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,18 +471,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,277 +807,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C34418C-4E89-40BF-9348-B310D91310AE}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:U11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
     <col min="5" max="5" width="9" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0.25" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.625" customWidth="1"/>
+    <col min="13" max="13" width="9" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="0.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21"/>
-      <c r="C2" s="26" t="s">
+    <row r="1" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="24"/>
+      <c r="C2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="I2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="27" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="L2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="O2" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="8">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="7">
         <v>360</v>
       </c>
       <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>1440</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="7">
+        <v>360</v>
+      </c>
+      <c r="I3" s="1">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
-        <f>C3*D3</f>
+      <c r="J3">
+        <f>H3*I3</f>
         <v>2880</v>
       </c>
-      <c r="F3" s="17">
+      <c r="K3" s="16">
         <v>360</v>
       </c>
-      <c r="G3" s="2">
+      <c r="L3">
         <v>8</v>
       </c>
-      <c r="H3" s="2">
-        <f>F3*G3</f>
+      <c r="M3">
+        <f>K3*L3</f>
         <v>2880</v>
       </c>
-      <c r="I3" s="16">
+      <c r="N3" s="15">
         <v>360</v>
       </c>
-      <c r="J3" s="7">
+      <c r="O3" s="6">
         <v>8</v>
       </c>
-      <c r="K3">
-        <f>I3*J3</f>
+      <c r="P3">
+        <f>N3*O3</f>
         <v>2880</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
-      <c r="C4" s="12">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="11">
+        <v>237.16</v>
+      </c>
+      <c r="D4" s="14">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>1185.8</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="11">
         <v>154.81</v>
       </c>
-      <c r="D4" s="15">
+      <c r="I4" s="14">
         <v>8</v>
       </c>
-      <c r="E4" s="14">
-        <f t="shared" ref="E4:E6" si="0">C4*D4</f>
+      <c r="J4" s="13">
+        <f t="shared" ref="J4:J6" si="0">H4*I4</f>
         <v>1238.48</v>
       </c>
-      <c r="F4" s="11">
+      <c r="K4" s="10">
         <v>154.81</v>
       </c>
-      <c r="G4" s="14">
+      <c r="L4" s="13">
         <v>8</v>
       </c>
-      <c r="H4" s="14">
-        <f t="shared" ref="H4:H7" si="1">F4*G4</f>
+      <c r="M4" s="13">
+        <f t="shared" ref="M4:M7" si="1">K4*L4</f>
         <v>1238.48</v>
       </c>
-      <c r="I4" s="12">
+      <c r="N4" s="11">
         <v>154.81</v>
       </c>
-      <c r="J4" s="15">
+      <c r="O4" s="14">
         <v>8</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K9" si="2">I4*J4</f>
+      <c r="P4">
+        <f t="shared" ref="P4:P9" si="2">N4*O4</f>
         <v>1238.48</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="9">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="25"/>
+      <c r="C5" s="8">
+        <v>108.42</v>
+      </c>
+      <c r="D5" s="9">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f>C5*D5</f>
+        <v>1084.2</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="8">
         <v>98.24</v>
       </c>
-      <c r="D5" s="10">
+      <c r="I5" s="9">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>785.92</v>
       </c>
-      <c r="F5" s="11">
+      <c r="K5" s="10">
         <v>98.24</v>
       </c>
-      <c r="G5" s="14">
+      <c r="L5" s="13">
         <v>8</v>
       </c>
-      <c r="H5" s="14">
+      <c r="M5" s="13">
         <f t="shared" si="1"/>
         <v>785.92</v>
       </c>
-      <c r="I5" s="12">
+      <c r="N5" s="11">
         <v>98.24</v>
       </c>
-      <c r="J5" s="13">
+      <c r="O5" s="12">
         <v>8</v>
       </c>
-      <c r="K5">
+      <c r="P5">
         <f t="shared" si="2"/>
         <v>785.92</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="22"/>
-      <c r="C6" s="9">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="25"/>
+      <c r="C6" s="8">
+        <v>98.24</v>
+      </c>
+      <c r="D6" s="9">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <f>C6*D6</f>
+        <v>1571.84</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="8">
         <v>58.24</v>
       </c>
-      <c r="D6" s="10">
+      <c r="I6" s="9">
         <v>12</v>
       </c>
-      <c r="E6" s="2">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>698.88</v>
       </c>
-      <c r="F6" s="11">
+      <c r="K6" s="10">
         <v>58.24</v>
       </c>
-      <c r="G6" s="14">
+      <c r="L6" s="13">
         <v>12</v>
       </c>
-      <c r="H6" s="14">
+      <c r="M6" s="13">
         <f t="shared" si="1"/>
         <v>698.88</v>
       </c>
-      <c r="I6" s="12">
+      <c r="N6" s="11">
         <v>58.24</v>
       </c>
-      <c r="J6" s="13">
+      <c r="O6" s="12">
         <v>12</v>
       </c>
-      <c r="K6">
+      <c r="P6">
         <f t="shared" si="2"/>
         <v>698.88</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="11">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="K7" s="10">
         <v>237.16</v>
       </c>
-      <c r="G7" s="14">
+      <c r="L7" s="13">
         <v>12</v>
       </c>
-      <c r="H7" s="14">
+      <c r="M7" s="13">
         <f t="shared" si="1"/>
         <v>2845.92</v>
       </c>
-      <c r="I7" s="12">
+      <c r="N7" s="11">
         <v>237.16</v>
       </c>
-      <c r="J7" s="13">
+      <c r="O7" s="12">
         <v>12</v>
       </c>
-      <c r="K7">
+      <c r="P7">
         <f t="shared" si="2"/>
         <v>2845.92</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="12">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="N8" s="11">
         <v>69.459999999999994</v>
       </c>
-      <c r="J8" s="13">
+      <c r="O8" s="12">
         <v>20</v>
       </c>
-      <c r="K8">
+      <c r="P8">
         <f t="shared" si="2"/>
         <v>1389.1999999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="12">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="25"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="N9" s="11">
         <v>58.24</v>
       </c>
-      <c r="J9" s="13">
+      <c r="O9" s="12">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="P9">
         <f t="shared" si="2"/>
         <v>582.4</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="23"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="2"/>
+    <row r="10" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="26"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18"/>
     </row>
-    <row r="11" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3">
         <f>SUM(E3:E11)</f>
+        <v>5281.84</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3">
+        <f>SUM(J3:J11)</f>
         <v>5603.28</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5">
-        <f>SUM(H3:H11)</f>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <f>SUM(M3:M11)</f>
         <v>8449.2000000000007</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4">
-        <f>SUM(K3:K11)</f>
+      <c r="M11" s="4"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="3">
+        <f>SUM(P3:P11)</f>
         <v>10420.800000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="G2:G10"/>
     <mergeCell ref="B2:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1085,6 +1153,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101005BE6623CB2330845AC24FF6A1A4121DC" ma:contentTypeVersion="3" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="efdf050c216e87091edb8a7115928d35">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="57514c1a-c392-4885-941b-31780aa76f68" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="43c6c558f5ebf6f3849d7b5eda44d27b" ns3:_="">
     <xsd:import namespace="57514c1a-c392-4885-941b-31780aa76f68"/>
@@ -1222,15 +1299,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1238,6 +1306,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9F6EC-574E-4BBB-95AF-6D5047C13163}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7155F23-4830-4CF0-9B2F-8DBDD1518ACB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1251,14 +1327,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9F6EC-574E-4BBB-95AF-6D5047C13163}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>